<commit_message>
Tracked down missing logs with ids and fixed minor things in viz
</commit_message>
<xml_diff>
--- a/analyzing_log/session_mega_id_writeout.xlsx
+++ b/analyzing_log/session_mega_id_writeout.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="session_mega_id_writeout_annota" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Session</t>
   </si>
@@ -88,6 +88,27 @@
   </si>
   <si>
     <t>2017-3-28_15.00.00 - 2017-3-28_17.00.00</t>
+  </si>
+  <si>
+    <t>total useable</t>
+  </si>
+  <si>
+    <t>total to recover</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>mismatch/missing</t>
+  </si>
+  <si>
+    <t>duplicated</t>
+  </si>
+  <si>
+    <t>(bad because pilot and missing graph logging events)</t>
+  </si>
+  <si>
+    <t>(bad because of commotion cuased from signing out computers)</t>
   </si>
 </sst>
 </file>
@@ -571,12 +592,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -898,13 +920,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF45"/>
+  <dimension ref="A1:AF50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="55.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -927,19 +952,19 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
       <c r="F2" s="1"/>
@@ -960,10 +985,15 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>5</v>
       </c>
       <c r="F3" s="1"/>
@@ -2127,19 +2157,19 @@
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>12</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>13</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>12</v>
       </c>
       <c r="F35" s="2"/>
@@ -2181,10 +2211,15 @@
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>9</v>
       </c>
       <c r="F36" s="2"/>
@@ -2236,7 +2271,7 @@
       <c r="G38">
         <v>12017165</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="3">
         <v>13578154</v>
       </c>
       <c r="I38">
@@ -2263,10 +2298,10 @@
       <c r="G39">
         <v>12017165</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="3">
         <v>13578154</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="3">
         <v>13578154</v>
       </c>
       <c r="J39">
@@ -2299,7 +2334,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="2"/>
-      <c r="G41">
+      <c r="G41" s="3">
         <v>15749160</v>
       </c>
       <c r="H41">
@@ -2320,10 +2355,10 @@
         <v>5</v>
       </c>
       <c r="F42" s="2"/>
-      <c r="G42">
+      <c r="G42" s="3">
         <v>15749160</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="3">
         <v>15749160</v>
       </c>
       <c r="I42">
@@ -2387,7 +2422,44 @@
         <v>19913165</v>
       </c>
     </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5">
+        <f>SUM(C5:C32)+SUM(E38+E41+E44)</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5">
+        <f>C38-E38+C41-E41+C44-E44</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>